<commit_message>
vault backup: 2025-11-25 18:32:06
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B9DE1C-E9E1-47F7-AD8C-9ABBB3BA6734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46C468C-A359-4DCA-80C9-6D37DF8CD7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -29,10 +29,6 @@
   </si>
   <si>
     <t>来访者姓名或代码</t>
-  </si>
-  <si>
-    <t>第四天
-日期:</t>
   </si>
   <si>
     <t>第五天
@@ -120,9 +116,6 @@
   </si>
   <si>
     <t>22：43</t>
-  </si>
-  <si>
-    <t>12：00</t>
   </si>
   <si>
     <t>无</t>
@@ -147,6 +140,22 @@
   </si>
   <si>
     <t>24：00</t>
+  </si>
+  <si>
+    <t>第四天
+日期:2025-11-25</t>
+  </si>
+  <si>
+    <t>23：00</t>
+  </si>
+  <si>
+    <t>8：33</t>
+  </si>
+  <si>
+    <t>8：40</t>
+  </si>
+  <si>
+    <t>22：20</t>
   </si>
 </sst>
 </file>
@@ -594,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -632,7 +641,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -644,102 +653,110 @@
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="33">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="16.5">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="16.5">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="16.5">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="49.5">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>40</v>
@@ -750,14 +767,16 @@
       <c r="D9" s="1">
         <v>10</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>30</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="16.5">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
@@ -768,14 +787,16 @@
       <c r="D10" s="1">
         <v>2</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>4</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="33">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1">
         <v>20</v>
@@ -786,14 +807,16 @@
       <c r="D11" s="1">
         <v>30</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>30</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="33">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>480</v>
@@ -804,32 +827,36 @@
       <c r="D12" s="1">
         <v>240</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>450</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="82.5">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="66">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1">
         <v>48</v>
@@ -840,14 +867,16 @@
       <c r="D14" s="1">
         <v>70</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>40</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="49.5">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
@@ -858,14 +887,16 @@
       <c r="D15" s="1">
         <v>4</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="99">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>4</v>
@@ -876,14 +907,16 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1">
+        <v>4</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="115.5">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1">
         <v>4</v>
@@ -894,25 +927,29 @@
       <c r="D17" s="1">
         <v>4</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>2</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="66">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>

</xml_diff>

<commit_message>
vault backup: 2025-11-26 13:32:36
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46C468C-A359-4DCA-80C9-6D37DF8CD7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A27C295-23D4-4333-BB07-7642DC2B0FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -29,10 +29,6 @@
   </si>
   <si>
     <t>来访者姓名或代码</t>
-  </si>
-  <si>
-    <t>第五天
-日期:</t>
   </si>
   <si>
     <t>第六天
@@ -139,9 +135,6 @@
 放松</t>
   </si>
   <si>
-    <t>24：00</t>
-  </si>
-  <si>
     <t>第四天
 日期:2025-11-25</t>
   </si>
@@ -156,6 +149,22 @@
   </si>
   <si>
     <t>22：20</t>
+  </si>
+  <si>
+    <t>第五天
+日期:2025-11-26</t>
+  </si>
+  <si>
+    <t>7：50</t>
+  </si>
+  <si>
+    <t>22：40</t>
+  </si>
+  <si>
+    <t>00：00</t>
+  </si>
+  <si>
+    <t>23：20</t>
   </si>
 </sst>
 </file>
@@ -603,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -641,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -653,110 +662,118 @@
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="33">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="16.5">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="16.5">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="16.5">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="49.5">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>40</v>
@@ -770,13 +787,15 @@
       <c r="E9" s="1">
         <v>30</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>50</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="16.5">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
@@ -790,13 +809,15 @@
       <c r="E10" s="1">
         <v>4</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="33">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>20</v>
@@ -810,13 +831,15 @@
       <c r="E11" s="1">
         <v>30</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>20</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="33">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>480</v>
@@ -830,33 +853,37 @@
       <c r="E12" s="1">
         <v>450</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1">
+        <v>420</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="82.5">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="66">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>48</v>
@@ -870,13 +897,15 @@
       <c r="E14" s="1">
         <v>40</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1">
+        <v>90</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="49.5">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
@@ -890,13 +919,15 @@
       <c r="E15" s="1">
         <v>3</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="99">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1">
         <v>4</v>
@@ -910,13 +941,15 @@
       <c r="E16" s="1">
         <v>4</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="115.5">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>4</v>
@@ -930,27 +963,31 @@
       <c r="E17" s="1">
         <v>2</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1">
+        <v>4</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="66">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>

</xml_diff>

<commit_message>
vault backup: 2025-11-27 14:31:33
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A27C295-23D4-4333-BB07-7642DC2B0FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A03366C-DBE5-48D9-A97E-5C97FC57AA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -29,10 +29,6 @@
   </si>
   <si>
     <t>来访者姓名或代码</t>
-  </si>
-  <si>
-    <t>第六天
-日期:</t>
   </si>
   <si>
     <t>第七天
@@ -115,10 +111,6 @@
   </si>
   <si>
     <t>无</t>
-  </si>
-  <si>
-    <t>您整晚的睡眠质量如何?
-0 1 2 3 4</t>
   </si>
   <si>
     <t>您昨晚睡前的身体紧张程度如何? 
@@ -165,6 +157,14 @@
   </si>
   <si>
     <t>23：20</t>
+  </si>
+  <si>
+    <t>第六天
+日期:2025-11-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">您整晚的睡眠质量如何?
+0很差 1 2 3 4很好 </t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -650,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -662,118 +662,126 @@
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="33">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="16.5">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="16.5">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="16.5">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="49.5">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>40</v>
@@ -790,12 +798,14 @@
       <c r="F9" s="1">
         <v>50</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>40</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="16.5">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
@@ -812,12 +822,14 @@
       <c r="F10" s="1">
         <v>3</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="33">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>20</v>
@@ -834,12 +846,14 @@
       <c r="F11" s="1">
         <v>20</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="33">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>480</v>
@@ -856,34 +870,38 @@
       <c r="F12" s="1">
         <v>420</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <v>480</v>
+      </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="82.5">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="66">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>48</v>
@@ -900,12 +918,14 @@
       <c r="F14" s="1">
         <v>90</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="1">
+        <v>40</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="49.5">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
@@ -922,12 +942,14 @@
       <c r="F15" s="1">
         <v>3</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1">
+        <v>4</v>
+      </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="99">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1">
         <v>4</v>
@@ -944,12 +966,14 @@
       <c r="F16" s="1">
         <v>1</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16" s="1">
+        <v>3</v>
+      </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="115.5">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1">
         <v>4</v>
@@ -966,29 +990,33 @@
       <c r="F17" s="1">
         <v>4</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="66">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="H18" s="1"/>
     </row>
     <row r="20" spans="1:8">

</xml_diff>

<commit_message>
vault backup: 2025-11-28 16:37:56
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A03366C-DBE5-48D9-A97E-5C97FC57AA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F2B75F-E780-41BB-8993-515E7DAE0CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -29,10 +29,6 @@
   </si>
   <si>
     <t>来访者姓名或代码</t>
-  </si>
-  <si>
-    <t>第七天
-日期:</t>
   </si>
   <si>
     <t>您今天早上几点醒来?</t>
@@ -165,6 +161,47 @@
   <si>
     <t xml:space="preserve">您整晚的睡眠质量如何?
 0很差 1 2 3 4很好 </t>
+  </si>
+  <si>
+    <t>第七天
+日期:2025-11-28</t>
+  </si>
+  <si>
+    <t>7：20</t>
+  </si>
+  <si>
+    <t>7：30</t>
+  </si>
+  <si>
+    <t>23：10</t>
+  </si>
+  <si>
+    <t>第一天
+日期:2025-11-29</t>
+  </si>
+  <si>
+    <t>第二天
+日期:2025-11-30</t>
+  </si>
+  <si>
+    <t>第三天
+日期:2025-12-1</t>
+  </si>
+  <si>
+    <t>第四天
+日期:2025-12-2</t>
+  </si>
+  <si>
+    <t>第五天
+日期:2025-12-3</t>
+  </si>
+  <si>
+    <t>第六天
+日期:2025-12-4</t>
+  </si>
+  <si>
+    <t>第七天
+日期:2025-12-5</t>
   </si>
 </sst>
 </file>
@@ -610,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -650,7 +687,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -662,126 +699,134 @@
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="33">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="16.5">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="16.5">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="16.5">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="49.5">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>40</v>
@@ -801,11 +846,13 @@
       <c r="G9" s="1">
         <v>40</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="16.5">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
@@ -825,11 +872,13 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="33">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>20</v>
@@ -849,11 +898,13 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="33">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>480</v>
@@ -873,35 +924,39 @@
       <c r="G12" s="1">
         <v>480</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>460</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="82.5">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="66">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>48</v>
@@ -921,11 +976,13 @@
       <c r="G14" s="1">
         <v>40</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="49.5">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
@@ -945,11 +1002,13 @@
       <c r="G15" s="1">
         <v>4</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="99">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1">
         <v>4</v>
@@ -969,11 +1028,13 @@
       <c r="G16" s="1">
         <v>3</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="115.5">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1">
         <v>4</v>
@@ -993,40 +1054,277 @@
       <c r="G17" s="1">
         <v>3</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="66">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3"/>
     </row>
+    <row r="21" spans="1:8" ht="22.5">
+      <c r="A21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="17.25">
+      <c r="A22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" ht="16.5">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:8" ht="54">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="33">
+      <c r="A25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" ht="16.5">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="16.5">
+      <c r="A27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="16.5">
+      <c r="A28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" ht="49.5">
+      <c r="A29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" ht="16.5">
+      <c r="A30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" ht="33">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" ht="33">
+      <c r="A32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" ht="82.5">
+      <c r="A33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" ht="66">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" ht="49.5">
+      <c r="A35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" ht="99">
+      <c r="A36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" ht="115.5">
+      <c r="A37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" ht="66">
+      <c r="A38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="B23:H23"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
vault backup: 2025-12-08 11:21:24
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F2B75F-E780-41BB-8993-515E7DAE0CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C404217F-E105-4054-B727-52E4C87EED06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -203,12 +203,97 @@
     <t>第七天
 日期:2025-12-5</t>
   </si>
+  <si>
+    <t>11：00</t>
+  </si>
+  <si>
+    <t>第一天
+日期:2025-12-06</t>
+  </si>
+  <si>
+    <t>第二天
+日期:2025-12-07</t>
+  </si>
+  <si>
+    <t>第三天
+日期:2025-12-08</t>
+  </si>
+  <si>
+    <t>第四天
+日期:2025-12-9</t>
+  </si>
+  <si>
+    <t>第五天
+日期:2025-12-10</t>
+  </si>
+  <si>
+    <t>第六天
+日期:2025-12-11</t>
+  </si>
+  <si>
+    <t>第七天
+日期:2025-12-12</t>
+  </si>
+  <si>
+    <t>7：14</t>
+  </si>
+  <si>
+    <t>24：00</t>
+  </si>
+  <si>
+    <t>24：20</t>
+  </si>
+  <si>
+    <t>24：30</t>
+  </si>
+  <si>
+    <t>22：00</t>
+  </si>
+  <si>
+    <t>22：50</t>
+  </si>
+  <si>
+    <t>7：27</t>
+  </si>
+  <si>
+    <t>23：40</t>
+  </si>
+  <si>
+    <t>6：46</t>
+  </si>
+  <si>
+    <t>23：30</t>
+  </si>
+  <si>
+    <t>8：12</t>
+  </si>
+  <si>
+    <t>6：04</t>
+  </si>
+  <si>
+    <t>9：00</t>
+  </si>
+  <si>
+    <t>24：10</t>
+  </si>
+  <si>
+    <t>7：23</t>
+  </si>
+  <si>
+    <t>9：30</t>
+  </si>
+  <si>
+    <t>10：00</t>
+  </si>
+  <si>
+    <t>有 30</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +325,11 @@
       <color rgb="FF808080"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="微软雅黑"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -255,7 +345,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -315,11 +405,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -328,6 +429,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -336,13 +446,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -647,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -659,42 +766,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1088,42 +1195,42 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" ht="16.5">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="10"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1153,172 +1260,685 @@
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="16.5">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="16.5">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="16.5">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="49.5">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="B29" s="1">
+        <v>20</v>
+      </c>
+      <c r="C29" s="1">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1">
+        <v>20</v>
+      </c>
+      <c r="G29" s="1">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="16.5">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="B30" s="1">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="33">
       <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="B31" s="1">
+        <v>14</v>
+      </c>
+      <c r="C31" s="1">
+        <v>5</v>
+      </c>
+      <c r="D31" s="1">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1">
+        <v>10</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="33">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="B32" s="1">
+        <v>480</v>
+      </c>
+      <c r="C32" s="1">
+        <v>420</v>
+      </c>
+      <c r="D32" s="1">
+        <v>450</v>
+      </c>
+      <c r="E32" s="1">
+        <v>480</v>
+      </c>
+      <c r="F32" s="1">
+        <v>400</v>
+      </c>
+      <c r="G32" s="1">
+        <v>430</v>
+      </c>
+      <c r="H32" s="1">
+        <v>280</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="82.5">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="66">
       <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="B34" s="1">
+        <v>30</v>
+      </c>
+      <c r="C34" s="1">
+        <v>60</v>
+      </c>
+      <c r="D34" s="1">
+        <v>40</v>
+      </c>
+      <c r="E34" s="1">
+        <v>15</v>
+      </c>
+      <c r="F34" s="1">
+        <v>10</v>
+      </c>
+      <c r="G34" s="1">
+        <v>40</v>
+      </c>
+      <c r="H34" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="49.5">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="B35" s="1">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>4</v>
+      </c>
+      <c r="H35" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="99">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="B36" s="1">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3</v>
+      </c>
+      <c r="E36" s="1">
+        <v>4</v>
+      </c>
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>3</v>
+      </c>
+      <c r="H36" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="115.5">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
+      <c r="B37" s="1">
+        <v>3</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3</v>
+      </c>
+      <c r="F37" s="1">
+        <v>4</v>
+      </c>
+      <c r="G37" s="1">
+        <v>4</v>
+      </c>
+      <c r="H37" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="66">
       <c r="A38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="22.5">
+      <c r="A40" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="1:8" ht="17.25">
+      <c r="A41" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" spans="1:8" ht="16.5">
+      <c r="A42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8" ht="54">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="33">
+      <c r="A44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" ht="16.5">
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" ht="16.5">
+      <c r="A46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" ht="16.5">
+      <c r="A47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" ht="49.5">
+      <c r="A48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="1">
+        <v>20</v>
+      </c>
+      <c r="C48" s="1">
+        <v>30</v>
+      </c>
+      <c r="D48" s="1">
+        <v>10</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" ht="16.5">
+      <c r="A49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" ht="33">
+      <c r="A50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" ht="33">
+      <c r="A51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="1">
+        <v>400</v>
+      </c>
+      <c r="C51" s="1">
+        <v>400</v>
+      </c>
+      <c r="D51" s="1">
+        <v>480</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" ht="82.5">
+      <c r="A52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" ht="66">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="1">
+        <v>40</v>
+      </c>
+      <c r="C53" s="1">
+        <v>30</v>
+      </c>
+      <c r="D53" s="1">
+        <v>30</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" ht="49.5">
+      <c r="A54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="1">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1">
+        <v>4</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" ht="99">
+      <c r="A55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" s="1">
+        <v>4</v>
+      </c>
+      <c r="C55" s="1">
+        <v>3</v>
+      </c>
+      <c r="D55" s="1">
+        <v>3</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:8" ht="115.5">
+      <c r="A56" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" s="1">
+        <v>4</v>
+      </c>
+      <c r="C56" s="1">
+        <v>4</v>
+      </c>
+      <c r="D56" s="1">
+        <v>4</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" ht="66">
+      <c r="A57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A1:H1"/>
@@ -1327,5 +1947,6 @@
     <mergeCell ref="A22:H22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2025-12-09 10:27:49
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C404217F-E105-4054-B727-52E4C87EED06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641FFBC6-C7CB-4D96-98A3-A881009F5C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="80">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -287,6 +287,12 @@
   </si>
   <si>
     <t>有 30</t>
+  </si>
+  <si>
+    <t>8：30</t>
+  </si>
+  <si>
+    <t>8：45</t>
   </si>
 </sst>
 </file>
@@ -429,6 +435,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -436,20 +456,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -757,7 +763,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -766,42 +772,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1195,42 +1201,42 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" ht="16.5">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="6"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1330,7 +1336,7 @@
       <c r="G27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1477,16 +1483,16 @@
       <c r="D33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E33" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H33" s="11" t="s">
+      <c r="E33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1621,42 +1627,42 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="9"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="8"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="9"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="8"/>
     </row>
     <row r="42" spans="1:8" ht="16.5">
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="6"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -1695,7 +1701,9 @@
       <c r="D44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -1713,7 +1721,9 @@
       <c r="D45" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -1731,7 +1741,9 @@
       <c r="D46" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -1749,7 +1761,9 @@
       <c r="D47" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E47" s="1"/>
+      <c r="E47" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -1767,7 +1781,9 @@
       <c r="D48" s="1">
         <v>10</v>
       </c>
-      <c r="E48" s="1"/>
+      <c r="E48" s="1">
+        <v>10</v>
+      </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -1785,7 +1801,9 @@
       <c r="D49" s="1">
         <v>0</v>
       </c>
-      <c r="E49" s="1"/>
+      <c r="E49" s="1">
+        <v>2</v>
+      </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -1803,7 +1821,9 @@
       <c r="D50" s="1">
         <v>0</v>
       </c>
-      <c r="E50" s="1"/>
+      <c r="E50" s="1">
+        <v>80</v>
+      </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -1821,7 +1841,9 @@
       <c r="D51" s="1">
         <v>480</v>
       </c>
-      <c r="E51" s="1"/>
+      <c r="E51" s="1">
+        <v>460</v>
+      </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -1839,7 +1861,9 @@
       <c r="D52" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="1"/>
+      <c r="E52" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -1857,7 +1881,9 @@
       <c r="D53" s="1">
         <v>30</v>
       </c>
-      <c r="E53" s="1"/>
+      <c r="E53" s="1">
+        <v>20</v>
+      </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -1875,7 +1901,9 @@
       <c r="D54" s="1">
         <v>3</v>
       </c>
-      <c r="E54" s="1"/>
+      <c r="E54" s="1">
+        <v>2</v>
+      </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -1893,7 +1921,9 @@
       <c r="D55" s="1">
         <v>3</v>
       </c>
-      <c r="E55" s="1"/>
+      <c r="E55" s="1">
+        <v>4</v>
+      </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -1911,7 +1941,9 @@
       <c r="D56" s="1">
         <v>4</v>
       </c>
-      <c r="E56" s="1"/>
+      <c r="E56" s="1">
+        <v>2</v>
+      </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -1929,22 +1961,24 @@
       <c r="D57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E57" s="1"/>
+      <c r="E57" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="B42:H42"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-10 10:18:21
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641FFBC6-C7CB-4D96-98A3-A881009F5C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D16B965-D5A1-4FC1-AF90-EAEC45039C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="80">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -426,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -446,9 +446,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -456,6 +453,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -762,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -784,7 +787,7 @@
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7"/>
@@ -799,15 +802,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1213,7 +1216,7 @@
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="7"/>
@@ -1228,15 +1231,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="12"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1639,7 +1642,7 @@
       <c r="H40" s="8"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="7"/>
@@ -1654,15 +1657,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="12"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="11"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -1704,7 +1707,9 @@
       <c r="E44" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F44" s="1"/>
+      <c r="F44" s="13">
+        <v>0.32083333333333336</v>
+      </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
     </row>
@@ -1724,7 +1729,9 @@
       <c r="E45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45" s="13">
+        <v>0.34027777777777779</v>
+      </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
     </row>
@@ -1744,7 +1751,9 @@
       <c r="E46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F46" s="1"/>
+      <c r="F46" s="13">
+        <v>0.96180555555555558</v>
+      </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
     </row>
@@ -1764,7 +1773,9 @@
       <c r="E47" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F47" s="1"/>
+      <c r="F47" s="13">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
@@ -1784,7 +1795,9 @@
       <c r="E48" s="1">
         <v>10</v>
       </c>
-      <c r="F48" s="1"/>
+      <c r="F48" s="1">
+        <v>20</v>
+      </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
     </row>
@@ -1804,7 +1817,9 @@
       <c r="E49" s="1">
         <v>2</v>
       </c>
-      <c r="F49" s="1"/>
+      <c r="F49" s="1">
+        <v>2</v>
+      </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
@@ -1824,7 +1839,9 @@
       <c r="E50" s="1">
         <v>80</v>
       </c>
-      <c r="F50" s="1"/>
+      <c r="F50" s="1">
+        <v>5</v>
+      </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
@@ -1844,7 +1861,9 @@
       <c r="E51" s="1">
         <v>460</v>
       </c>
-      <c r="F51" s="1"/>
+      <c r="F51" s="1">
+        <v>480</v>
+      </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
@@ -1864,7 +1883,9 @@
       <c r="E52" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F52" s="1"/>
+      <c r="F52" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
@@ -1884,7 +1905,9 @@
       <c r="E53" s="1">
         <v>20</v>
       </c>
-      <c r="F53" s="1"/>
+      <c r="F53" s="1">
+        <v>35</v>
+      </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
@@ -1904,7 +1927,9 @@
       <c r="E54" s="1">
         <v>2</v>
       </c>
-      <c r="F54" s="1"/>
+      <c r="F54" s="1">
+        <v>3</v>
+      </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
     </row>
@@ -1924,7 +1949,9 @@
       <c r="E55" s="1">
         <v>4</v>
       </c>
-      <c r="F55" s="1"/>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
@@ -1944,7 +1971,9 @@
       <c r="E56" s="1">
         <v>2</v>
       </c>
-      <c r="F56" s="1"/>
+      <c r="F56" s="1">
+        <v>2</v>
+      </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
@@ -1964,21 +1993,23 @@
       <c r="E57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F57" s="1"/>
+      <c r="F57" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A2:H2"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-11 10:48:04
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D16B965-D5A1-4FC1-AF90-EAEC45039C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A200EAF-F5E5-46EF-984F-950ACEA9C771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="80">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -441,7 +441,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -455,11 +458,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -766,7 +766,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -775,42 +775,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1204,42 +1204,42 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" ht="16.5">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1630,42 +1630,42 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8" ht="16.5">
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -1707,10 +1707,12 @@
       <c r="E44" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F44" s="13">
+      <c r="F44" s="6">
         <v>0.32083333333333336</v>
       </c>
-      <c r="G44" s="1"/>
+      <c r="G44" s="6">
+        <v>0.32083333333333336</v>
+      </c>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" ht="16.5">
@@ -1729,10 +1731,12 @@
       <c r="E45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F45" s="13">
+      <c r="F45" s="6">
         <v>0.34027777777777779</v>
       </c>
-      <c r="G45" s="1"/>
+      <c r="G45" s="6">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" ht="16.5">
@@ -1751,10 +1755,12 @@
       <c r="E46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F46" s="13">
+      <c r="F46" s="6">
         <v>0.96180555555555558</v>
       </c>
-      <c r="G46" s="1"/>
+      <c r="G46" s="6">
+        <v>0.96180555555555558</v>
+      </c>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" ht="16.5">
@@ -1773,10 +1779,12 @@
       <c r="E47" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F47" s="13">
+      <c r="F47" s="6">
         <v>0.97222222222222221</v>
       </c>
-      <c r="G47" s="1"/>
+      <c r="G47" s="6">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" ht="49.5">
@@ -1798,7 +1806,9 @@
       <c r="F48" s="1">
         <v>20</v>
       </c>
-      <c r="G48" s="1"/>
+      <c r="G48" s="1">
+        <v>10</v>
+      </c>
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" ht="16.5">
@@ -1820,7 +1830,9 @@
       <c r="F49" s="1">
         <v>2</v>
       </c>
-      <c r="G49" s="1"/>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" ht="33">
@@ -1842,7 +1854,9 @@
       <c r="F50" s="1">
         <v>5</v>
       </c>
-      <c r="G50" s="1"/>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" ht="33">
@@ -1864,7 +1878,9 @@
       <c r="F51" s="1">
         <v>480</v>
       </c>
-      <c r="G51" s="1"/>
+      <c r="G51" s="1">
+        <v>510</v>
+      </c>
       <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8" ht="82.5">
@@ -1886,7 +1902,9 @@
       <c r="F52" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G52" s="1"/>
+      <c r="G52" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8" ht="66">
@@ -1908,7 +1926,9 @@
       <c r="F53" s="1">
         <v>35</v>
       </c>
-      <c r="G53" s="1"/>
+      <c r="G53" s="1">
+        <v>15</v>
+      </c>
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" ht="49.5">
@@ -1930,7 +1950,9 @@
       <c r="F54" s="1">
         <v>3</v>
       </c>
-      <c r="G54" s="1"/>
+      <c r="G54" s="1">
+        <v>4</v>
+      </c>
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" ht="99">
@@ -1952,7 +1974,9 @@
       <c r="F55" s="1">
         <v>1</v>
       </c>
-      <c r="G55" s="1"/>
+      <c r="G55" s="1">
+        <v>3</v>
+      </c>
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" ht="115.5">
@@ -1974,7 +1998,9 @@
       <c r="F56" s="1">
         <v>2</v>
       </c>
-      <c r="G56" s="1"/>
+      <c r="G56" s="1">
+        <v>3</v>
+      </c>
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" ht="66">
@@ -1996,7 +2022,9 @@
       <c r="F57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G57" s="1"/>
+      <c r="G57" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H57" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2025-12-12 11:37:09
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A200EAF-F5E5-46EF-984F-950ACEA9C771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559C8960-5D75-47BC-92B1-4EEBE972ACC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="90">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -293,6 +293,43 @@
   </si>
   <si>
     <t>8：45</t>
+  </si>
+  <si>
+    <t>7：04</t>
+  </si>
+  <si>
+    <t>7：24</t>
+  </si>
+  <si>
+    <t>24：40</t>
+  </si>
+  <si>
+    <t>第一天
+日期:2025-12-13</t>
+  </si>
+  <si>
+    <t>第二天
+日期:2025-12-14</t>
+  </si>
+  <si>
+    <t>第三天
+日期:2025-12-15</t>
+  </si>
+  <si>
+    <t>第四天
+日期:2025-12-16</t>
+  </si>
+  <si>
+    <t>第五天
+日期:2025-12-17</t>
+  </si>
+  <si>
+    <t>第六天
+日期:2025-12-18</t>
+  </si>
+  <si>
+    <t>第七天
+日期:2025-12-19</t>
   </si>
 </sst>
 </file>
@@ -763,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1713,7 +1750,9 @@
       <c r="G44" s="6">
         <v>0.32083333333333336</v>
       </c>
-      <c r="H44" s="1"/>
+      <c r="H44" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="45" spans="1:8" ht="16.5">
       <c r="A45" s="1" t="s">
@@ -1737,7 +1776,9 @@
       <c r="G45" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="H45" s="1"/>
+      <c r="H45" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="46" spans="1:8" ht="16.5">
       <c r="A46" s="1" t="s">
@@ -1761,7 +1802,9 @@
       <c r="G46" s="6">
         <v>0.96180555555555558</v>
       </c>
-      <c r="H46" s="1"/>
+      <c r="H46" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="47" spans="1:8" ht="16.5">
       <c r="A47" s="1" t="s">
@@ -1785,7 +1828,9 @@
       <c r="G47" s="6">
         <v>0.96527777777777779</v>
       </c>
-      <c r="H47" s="1"/>
+      <c r="H47" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="48" spans="1:8" ht="49.5">
       <c r="A48" s="1" t="s">
@@ -1809,7 +1854,9 @@
       <c r="G48" s="1">
         <v>10</v>
       </c>
-      <c r="H48" s="1"/>
+      <c r="H48" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" spans="1:8" ht="16.5">
       <c r="A49" s="1" t="s">
@@ -1833,7 +1880,9 @@
       <c r="G49" s="1">
         <v>0</v>
       </c>
-      <c r="H49" s="1"/>
+      <c r="H49" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:8" ht="33">
       <c r="A50" s="1" t="s">
@@ -1857,7 +1906,9 @@
       <c r="G50" s="1">
         <v>0</v>
       </c>
-      <c r="H50" s="1"/>
+      <c r="H50" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="51" spans="1:8" ht="33">
       <c r="A51" s="1" t="s">
@@ -1881,7 +1932,9 @@
       <c r="G51" s="1">
         <v>510</v>
       </c>
-      <c r="H51" s="1"/>
+      <c r="H51" s="1">
+        <v>360</v>
+      </c>
     </row>
     <row r="52" spans="1:8" ht="82.5">
       <c r="A52" s="1" t="s">
@@ -1905,7 +1958,9 @@
       <c r="G52" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H52" s="1"/>
+      <c r="H52" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="53" spans="1:8" ht="66">
       <c r="A53" s="1" t="s">
@@ -1929,7 +1984,9 @@
       <c r="G53" s="1">
         <v>15</v>
       </c>
-      <c r="H53" s="1"/>
+      <c r="H53" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="54" spans="1:8" ht="49.5">
       <c r="A54" s="1" t="s">
@@ -1953,7 +2010,9 @@
       <c r="G54" s="1">
         <v>4</v>
       </c>
-      <c r="H54" s="1"/>
+      <c r="H54" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="55" spans="1:8" ht="99">
       <c r="A55" s="1" t="s">
@@ -1977,7 +2036,9 @@
       <c r="G55" s="1">
         <v>3</v>
       </c>
-      <c r="H55" s="1"/>
+      <c r="H55" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="56" spans="1:8" ht="115.5">
       <c r="A56" s="1" t="s">
@@ -2001,7 +2062,9 @@
       <c r="G56" s="1">
         <v>3</v>
       </c>
-      <c r="H56" s="1"/>
+      <c r="H56" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="57" spans="1:8" ht="66">
       <c r="A57" s="1" t="s">
@@ -2025,10 +2088,245 @@
       <c r="G57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H57" s="1"/>
+      <c r="H57" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="22.5">
+      <c r="A59" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="9"/>
+    </row>
+    <row r="60" spans="1:8" ht="17.25">
+      <c r="A60" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="9"/>
+    </row>
+    <row r="61" spans="1:8" ht="16.5">
+      <c r="A61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="12"/>
+    </row>
+    <row r="62" spans="1:8" ht="54">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="33">
+      <c r="A63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8" ht="16.5">
+      <c r="A64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" ht="16.5">
+      <c r="A65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" ht="16.5">
+      <c r="A66" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" ht="49.5">
+      <c r="A67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" ht="16.5">
+      <c r="A68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" ht="33">
+      <c r="A69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" ht="33">
+      <c r="A70" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" ht="82.5">
+      <c r="A71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+    </row>
+    <row r="72" spans="1:8" ht="66">
+      <c r="A72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+    </row>
+    <row r="73" spans="1:8" ht="49.5">
+      <c r="A73" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+    </row>
+    <row r="74" spans="1:8" ht="99">
+      <c r="A74" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" ht="115.5">
+      <c r="A75" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" ht="66">
+      <c r="A76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="B61:H61"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="B42:H42"/>
     <mergeCell ref="B23:H23"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-15 09:59:19
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559C8960-5D75-47BC-92B1-4EEBE972ACC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F20B2D1-3C56-4B0B-953C-5BB953BD7487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="94">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -330,6 +330,18 @@
   <si>
     <t>第七天
 日期:2025-12-19</t>
+  </si>
+  <si>
+    <t>8：14</t>
+  </si>
+  <si>
+    <t>22：30</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>上床后30 min</t>
   </si>
 </sst>
 </file>
@@ -481,11 +493,14 @@
     <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -494,9 +509,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -812,7 +824,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
@@ -824,7 +836,7 @@
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
@@ -839,15 +851,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1241,7 +1253,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="8"/>
@@ -1253,7 +1265,7 @@
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="8"/>
@@ -1268,15 +1280,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1667,7 +1679,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="8"/>
@@ -1679,7 +1691,7 @@
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="8"/>
@@ -1694,15 +1706,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2093,7 +2105,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="8"/>
@@ -2105,7 +2117,7 @@
       <c r="H59" s="9"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="8"/>
@@ -2120,15 +2132,15 @@
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2158,9 +2170,15 @@
       <c r="A63" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
+      <c r="B63" s="6">
+        <v>0.28472222222222221</v>
+      </c>
+      <c r="C63" s="6">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="E63" s="1"/>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
@@ -2170,9 +2188,15 @@
       <c r="A64" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
+      <c r="B64" s="6">
+        <v>0.28472222222222221</v>
+      </c>
+      <c r="C64" s="6">
+        <v>0.4375</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E64" s="1"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
@@ -2182,9 +2206,15 @@
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
+      <c r="B65" s="6">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C65" s="6">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E65" s="1"/>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
@@ -2194,9 +2224,15 @@
       <c r="A66" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="B66" s="6">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="C66" s="6">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="E66" s="1"/>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
@@ -2206,9 +2242,15 @@
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
+      <c r="B67" s="1">
+        <v>30</v>
+      </c>
+      <c r="C67" s="1">
+        <v>3</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -2218,9 +2260,15 @@
       <c r="A68" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
+      <c r="B68" s="1">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1">
+        <v>2</v>
+      </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -2230,9 +2278,15 @@
       <c r="A69" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+      <c r="B69" s="1">
+        <v>0</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1">
+        <v>65</v>
+      </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -2242,9 +2296,15 @@
       <c r="A70" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
+      <c r="B70" s="1">
+        <v>410</v>
+      </c>
+      <c r="C70" s="1">
+        <v>420</v>
+      </c>
+      <c r="D70" s="1">
+        <v>480</v>
+      </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -2254,9 +2314,15 @@
       <c r="A71" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -2266,9 +2332,15 @@
       <c r="A72" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
+      <c r="B72" s="1">
+        <v>60</v>
+      </c>
+      <c r="C72" s="1">
+        <v>2</v>
+      </c>
+      <c r="D72" s="1">
+        <v>30</v>
+      </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -2278,9 +2350,15 @@
       <c r="A73" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
+      <c r="B73" s="1">
+        <v>3</v>
+      </c>
+      <c r="C73" s="1">
+        <v>2</v>
+      </c>
+      <c r="D73" s="1">
+        <v>2</v>
+      </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -2290,9 +2368,15 @@
       <c r="A74" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
+      <c r="B74" s="1">
+        <v>3</v>
+      </c>
+      <c r="C74" s="1">
+        <v>2</v>
+      </c>
+      <c r="D74" s="1">
+        <v>4</v>
+      </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -2302,9 +2386,15 @@
       <c r="A75" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
+      <c r="B75" s="1">
+        <v>2</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1</v>
+      </c>
+      <c r="D75" s="1">
+        <v>1</v>
+      </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -2314,9 +2404,15 @@
       <c r="A76" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
+      <c r="B76" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -2324,18 +2420,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="A40:H40"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-17 11:11:31
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F20B2D1-3C56-4B0B-953C-5BB953BD7487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85DE676-A17A-4D32-98FC-4D5580A34EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="95">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>上床后30 min</t>
+  </si>
+  <si>
+    <t>7：42</t>
   </si>
 </sst>
 </file>
@@ -498,9 +501,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -509,6 +509,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -836,7 +839,7 @@
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
@@ -851,15 +854,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1265,7 +1268,7 @@
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="8"/>
@@ -1280,15 +1283,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1691,7 +1694,7 @@
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="8"/>
@@ -1706,15 +1709,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="13"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2117,7 +2120,7 @@
       <c r="H59" s="9"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="8"/>
@@ -2132,15 +2135,15 @@
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="13"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="12"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2180,7 +2183,9 @@
         <v>90</v>
       </c>
       <c r="E63" s="1"/>
-      <c r="F63" s="6"/>
+      <c r="F63" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="G63" s="6"/>
       <c r="H63" s="1"/>
     </row>
@@ -2198,7 +2203,9 @@
         <v>17</v>
       </c>
       <c r="E64" s="1"/>
-      <c r="F64" s="6"/>
+      <c r="F64" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G64" s="6"/>
       <c r="H64" s="1"/>
     </row>
@@ -2216,7 +2223,9 @@
         <v>91</v>
       </c>
       <c r="E65" s="1"/>
-      <c r="F65" s="6"/>
+      <c r="F65" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G65" s="6"/>
       <c r="H65" s="1"/>
     </row>
@@ -2234,7 +2243,9 @@
         <v>92</v>
       </c>
       <c r="E66" s="1"/>
-      <c r="F66" s="6"/>
+      <c r="F66" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="G66" s="6"/>
       <c r="H66" s="1"/>
     </row>
@@ -2252,7 +2263,9 @@
         <v>93</v>
       </c>
       <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
+      <c r="F67" s="1">
+        <v>30</v>
+      </c>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
     </row>
@@ -2269,8 +2282,12 @@
       <c r="D68" s="1">
         <v>2</v>
       </c>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1">
+        <v>2</v>
+      </c>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
     </row>
@@ -2287,8 +2304,12 @@
       <c r="D69" s="1">
         <v>65</v>
       </c>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
+      <c r="E69" s="1">
+        <v>60</v>
+      </c>
+      <c r="F69" s="1">
+        <v>5</v>
+      </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
     </row>
@@ -2306,7 +2327,9 @@
         <v>480</v>
       </c>
       <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+      <c r="F70" s="1">
+        <v>460</v>
+      </c>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
     </row>
@@ -2323,8 +2346,12 @@
       <c r="D71" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
+      <c r="E71" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
     </row>
@@ -2341,8 +2368,12 @@
       <c r="D72" s="1">
         <v>30</v>
       </c>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
+      <c r="E72" s="1">
+        <v>10</v>
+      </c>
+      <c r="F72" s="1">
+        <v>40</v>
+      </c>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
     </row>
@@ -2359,8 +2390,12 @@
       <c r="D73" s="1">
         <v>2</v>
       </c>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
+      <c r="E73" s="1">
+        <v>2</v>
+      </c>
+      <c r="F73" s="1">
+        <v>2</v>
+      </c>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
     </row>
@@ -2377,8 +2412,12 @@
       <c r="D74" s="1">
         <v>4</v>
       </c>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+      <c r="E74" s="1">
+        <v>3</v>
+      </c>
+      <c r="F74" s="1">
+        <v>4</v>
+      </c>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
     </row>
@@ -2395,8 +2434,12 @@
       <c r="D75" s="1">
         <v>1</v>
       </c>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
+      <c r="E75" s="1">
+        <v>2</v>
+      </c>
+      <c r="F75" s="1">
+        <v>2</v>
+      </c>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
     </row>
@@ -2413,13 +2456,22 @@
       <c r="D76" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
+      <c r="E76" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="A2:H2"/>
@@ -2427,11 +2479,6 @@
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-17 12:49:24
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85DE676-A17A-4D32-98FC-4D5580A34EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2234FEA-F2C5-41BC-AB6F-3864C3133CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="95">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -501,6 +501,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -509,9 +512,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -839,7 +839,7 @@
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
@@ -854,15 +854,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1268,7 +1268,7 @@
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="8"/>
@@ -1283,15 +1283,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1694,7 +1694,7 @@
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="8"/>
@@ -1709,15 +1709,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2120,7 +2120,7 @@
       <c r="H59" s="9"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="8"/>
@@ -2135,15 +2135,15 @@
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2182,7 +2182,9 @@
       <c r="D63" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E63" s="1"/>
+      <c r="E63" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F63" s="6" t="s">
         <v>94</v>
       </c>
@@ -2202,7 +2204,9 @@
       <c r="D64" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="1"/>
+      <c r="E64" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="F64" s="6" t="s">
         <v>15</v>
       </c>
@@ -2222,7 +2226,9 @@
       <c r="D65" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E65" s="1"/>
+      <c r="E65" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="F65" s="6" t="s">
         <v>38</v>
       </c>
@@ -2242,7 +2248,9 @@
       <c r="D66" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E66" s="1"/>
+      <c r="E66" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="F66" s="6" t="s">
         <v>69</v>
       </c>
@@ -2262,7 +2270,9 @@
       <c r="D67" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E67" s="1"/>
+      <c r="E67" s="1">
+        <v>25</v>
+      </c>
       <c r="F67" s="1">
         <v>30</v>
       </c>
@@ -2326,7 +2336,9 @@
       <c r="D70" s="1">
         <v>480</v>
       </c>
-      <c r="E70" s="1"/>
+      <c r="E70" s="1">
+        <v>480</v>
+      </c>
       <c r="F70" s="1">
         <v>460</v>
       </c>
@@ -2467,11 +2479,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="A2:H2"/>
@@ -2479,6 +2486,11 @@
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-18 12:21:02
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2234FEA-F2C5-41BC-AB6F-3864C3133CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7DDA85-CC89-4D91-BB97-FDE007122414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="95">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -501,9 +501,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -512,6 +509,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -839,7 +839,7 @@
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
@@ -854,15 +854,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1268,7 +1268,7 @@
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="8"/>
@@ -1283,15 +1283,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1694,7 +1694,7 @@
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="8"/>
@@ -1709,15 +1709,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="13"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2120,7 +2120,7 @@
       <c r="H59" s="9"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="8"/>
@@ -2135,15 +2135,15 @@
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="13"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="12"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2188,7 +2188,9 @@
       <c r="F63" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G63" s="6"/>
+      <c r="G63" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:8" ht="16.5">
@@ -2210,7 +2212,9 @@
       <c r="F64" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G64" s="6"/>
+      <c r="G64" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="1:8" ht="16.5">
@@ -2232,7 +2236,9 @@
       <c r="F65" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G65" s="6"/>
+      <c r="G65" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" ht="16.5">
@@ -2254,7 +2260,9 @@
       <c r="F66" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G66" s="6"/>
+      <c r="G66" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="H66" s="1"/>
     </row>
     <row r="67" spans="1:8" ht="49.5">
@@ -2276,7 +2284,9 @@
       <c r="F67" s="1">
         <v>30</v>
       </c>
-      <c r="G67" s="1"/>
+      <c r="G67" s="1">
+        <v>0</v>
+      </c>
       <c r="H67" s="1"/>
     </row>
     <row r="68" spans="1:8" ht="16.5">
@@ -2298,7 +2308,9 @@
       <c r="F68" s="1">
         <v>2</v>
       </c>
-      <c r="G68" s="1"/>
+      <c r="G68" s="1">
+        <v>0</v>
+      </c>
       <c r="H68" s="1"/>
     </row>
     <row r="69" spans="1:8" ht="33">
@@ -2320,7 +2332,9 @@
       <c r="F69" s="1">
         <v>5</v>
       </c>
-      <c r="G69" s="1"/>
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
       <c r="H69" s="1"/>
     </row>
     <row r="70" spans="1:8" ht="33">
@@ -2342,7 +2356,9 @@
       <c r="F70" s="1">
         <v>460</v>
       </c>
-      <c r="G70" s="1"/>
+      <c r="G70" s="1">
+        <v>540</v>
+      </c>
       <c r="H70" s="1"/>
     </row>
     <row r="71" spans="1:8" ht="82.5">
@@ -2364,7 +2380,9 @@
       <c r="F71" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G71" s="1"/>
+      <c r="G71" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" ht="66">
@@ -2386,7 +2404,9 @@
       <c r="F72" s="1">
         <v>40</v>
       </c>
-      <c r="G72" s="1"/>
+      <c r="G72" s="1">
+        <v>0</v>
+      </c>
       <c r="H72" s="1"/>
     </row>
     <row r="73" spans="1:8" ht="49.5">
@@ -2408,7 +2428,9 @@
       <c r="F73" s="1">
         <v>2</v>
       </c>
-      <c r="G73" s="1"/>
+      <c r="G73" s="1">
+        <v>4</v>
+      </c>
       <c r="H73" s="1"/>
     </row>
     <row r="74" spans="1:8" ht="99">
@@ -2430,7 +2452,9 @@
       <c r="F74" s="1">
         <v>4</v>
       </c>
-      <c r="G74" s="1"/>
+      <c r="G74" s="1">
+        <v>4</v>
+      </c>
       <c r="H74" s="1"/>
     </row>
     <row r="75" spans="1:8" ht="115.5">
@@ -2452,7 +2476,9 @@
       <c r="F75" s="1">
         <v>2</v>
       </c>
-      <c r="G75" s="1"/>
+      <c r="G75" s="1">
+        <v>3</v>
+      </c>
       <c r="H75" s="1"/>
     </row>
     <row r="76" spans="1:8" ht="66">
@@ -2474,11 +2500,18 @@
       <c r="F76" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G76" s="1"/>
+      <c r="G76" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H76" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="A2:H2"/>
@@ -2486,11 +2519,6 @@
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-19 09:00:33
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7DDA85-CC89-4D91-BB97-FDE007122414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BA95E1-EA37-48C4-AD34-7E81996CB35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="97">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>7：42</t>
+  </si>
+  <si>
+    <t>6：52</t>
+  </si>
+  <si>
+    <t>23：05</t>
   </si>
 </sst>
 </file>
@@ -501,6 +507,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -509,9 +518,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -817,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -839,7 +845,7 @@
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
@@ -854,15 +860,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1268,7 +1274,7 @@
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="8"/>
@@ -1283,15 +1289,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1694,7 +1700,7 @@
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="8"/>
@@ -1709,15 +1715,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2120,7 +2126,7 @@
       <c r="H59" s="9"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="8"/>
@@ -2135,15 +2141,15 @@
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2191,7 +2197,9 @@
       <c r="G63" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="1"/>
+      <c r="H63" s="6">
+        <v>0.28611111111111109</v>
+      </c>
     </row>
     <row r="64" spans="1:8" ht="16.5">
       <c r="A64" s="1" t="s">
@@ -2215,7 +2223,9 @@
       <c r="G64" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H64" s="1"/>
+      <c r="H64" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="65" spans="1:8" ht="16.5">
       <c r="A65" s="1" t="s">
@@ -2239,7 +2249,9 @@
       <c r="G65" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H65" s="1"/>
+      <c r="H65" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="66" spans="1:8" ht="16.5">
       <c r="A66" s="1" t="s">
@@ -2263,7 +2275,9 @@
       <c r="G66" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H66" s="1"/>
+      <c r="H66" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="67" spans="1:8" ht="49.5">
       <c r="A67" s="1" t="s">
@@ -2287,7 +2301,9 @@
       <c r="G67" s="1">
         <v>0</v>
       </c>
-      <c r="H67" s="1"/>
+      <c r="H67" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="68" spans="1:8" ht="16.5">
       <c r="A68" s="1" t="s">
@@ -2311,7 +2327,9 @@
       <c r="G68" s="1">
         <v>0</v>
       </c>
-      <c r="H68" s="1"/>
+      <c r="H68" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:8" ht="33">
       <c r="A69" s="1" t="s">
@@ -2335,7 +2353,9 @@
       <c r="G69" s="1">
         <v>0</v>
       </c>
-      <c r="H69" s="1"/>
+      <c r="H69" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="70" spans="1:8" ht="33">
       <c r="A70" s="1" t="s">
@@ -2359,7 +2379,9 @@
       <c r="G70" s="1">
         <v>540</v>
       </c>
-      <c r="H70" s="1"/>
+      <c r="H70" s="1">
+        <v>440</v>
+      </c>
     </row>
     <row r="71" spans="1:8" ht="82.5">
       <c r="A71" s="1" t="s">
@@ -2383,7 +2405,9 @@
       <c r="G71" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H71" s="1"/>
+      <c r="H71" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="72" spans="1:8" ht="66">
       <c r="A72" s="1" t="s">
@@ -2407,7 +2431,9 @@
       <c r="G72" s="1">
         <v>0</v>
       </c>
-      <c r="H72" s="1"/>
+      <c r="H72" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="73" spans="1:8" ht="49.5">
       <c r="A73" s="1" t="s">
@@ -2431,7 +2457,9 @@
       <c r="G73" s="1">
         <v>4</v>
       </c>
-      <c r="H73" s="1"/>
+      <c r="H73" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="74" spans="1:8" ht="99">
       <c r="A74" s="1" t="s">
@@ -2455,7 +2483,9 @@
       <c r="G74" s="1">
         <v>4</v>
       </c>
-      <c r="H74" s="1"/>
+      <c r="H74" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="75" spans="1:8" ht="115.5">
       <c r="A75" s="1" t="s">
@@ -2479,7 +2509,9 @@
       <c r="G75" s="1">
         <v>3</v>
       </c>
-      <c r="H75" s="1"/>
+      <c r="H75" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="76" spans="1:8" ht="66">
       <c r="A76" s="1" t="s">
@@ -2503,15 +2535,12 @@
       <c r="G76" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H76" s="1"/>
+      <c r="H76" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="A2:H2"/>
@@ -2519,6 +2548,11 @@
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-22 11:51:27
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BA95E1-EA37-48C4-AD34-7E81996CB35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3EBEBF-74B2-4FE2-8307-30BDD7E7BE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="109">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -351,6 +351,49 @@
   </si>
   <si>
     <t>23：05</t>
+  </si>
+  <si>
+    <t>第一天
+日期:2025-12-20</t>
+  </si>
+  <si>
+    <t>第二天
+日期:2025-12-21</t>
+  </si>
+  <si>
+    <t>第三天
+日期:2025-12-22</t>
+  </si>
+  <si>
+    <t>第四天
+日期:2025-12-23</t>
+  </si>
+  <si>
+    <t>第五天
+日期:2025-12-24</t>
+  </si>
+  <si>
+    <t>第六天
+日期:2025-12-25</t>
+  </si>
+  <si>
+    <t>第七天
+日期:2025-12-26</t>
+  </si>
+  <si>
+    <t>7：41</t>
+  </si>
+  <si>
+    <t>22：45</t>
+  </si>
+  <si>
+    <t>8：05</t>
+  </si>
+  <si>
+    <t>8：10</t>
+  </si>
+  <si>
+    <t>有 30 min</t>
   </si>
 </sst>
 </file>
@@ -507,9 +550,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -518,6 +558,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -821,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -845,7 +888,7 @@
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
@@ -860,15 +903,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1274,7 +1317,7 @@
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="8"/>
@@ -1289,15 +1332,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1700,7 +1743,7 @@
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="8"/>
@@ -1715,15 +1758,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="13"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2126,7 +2169,7 @@
       <c r="H59" s="9"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="8"/>
@@ -2141,15 +2184,15 @@
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="13"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="12"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2539,8 +2582,317 @@
         <v>26</v>
       </c>
     </row>
+    <row r="79" spans="1:8" ht="17.25">
+      <c r="A79" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="9"/>
+    </row>
+    <row r="80" spans="1:8" ht="16.5">
+      <c r="A80" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="12"/>
+    </row>
+    <row r="81" spans="1:8" ht="54">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="33">
+      <c r="A82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E82" s="1"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+    </row>
+    <row r="83" spans="1:8" ht="16.5">
+      <c r="A83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E83" s="1"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="1"/>
+    </row>
+    <row r="84" spans="1:8" ht="16.5">
+      <c r="A84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E84" s="1"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="1"/>
+    </row>
+    <row r="85" spans="1:8" ht="16.5">
+      <c r="A85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D85" s="6">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="E85" s="1"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="1"/>
+    </row>
+    <row r="86" spans="1:8" ht="49.5">
+      <c r="A86" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0</v>
+      </c>
+      <c r="C86" s="1">
+        <v>10</v>
+      </c>
+      <c r="D86" s="1">
+        <v>5</v>
+      </c>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+    </row>
+    <row r="87" spans="1:8" ht="16.5">
+      <c r="A87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0</v>
+      </c>
+      <c r="C87" s="1">
+        <v>0</v>
+      </c>
+      <c r="D87" s="1">
+        <v>1</v>
+      </c>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+    </row>
+    <row r="88" spans="1:8" ht="33">
+      <c r="A88" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0</v>
+      </c>
+      <c r="C88" s="1">
+        <v>0</v>
+      </c>
+      <c r="D88" s="1">
+        <v>3</v>
+      </c>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+    </row>
+    <row r="89" spans="1:8" ht="33">
+      <c r="A89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" s="1">
+        <v>540</v>
+      </c>
+      <c r="C89" s="1">
+        <v>540</v>
+      </c>
+      <c r="D89" s="1">
+        <v>480</v>
+      </c>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+    </row>
+    <row r="90" spans="1:8" ht="82.5">
+      <c r="A90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+    </row>
+    <row r="91" spans="1:8" ht="66">
+      <c r="A91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0</v>
+      </c>
+      <c r="C91" s="1">
+        <v>10</v>
+      </c>
+      <c r="D91" s="1">
+        <v>25</v>
+      </c>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+    </row>
+    <row r="92" spans="1:8" ht="49.5">
+      <c r="A92" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92" s="1">
+        <v>4</v>
+      </c>
+      <c r="C92" s="1">
+        <v>4</v>
+      </c>
+      <c r="D92" s="1">
+        <v>4</v>
+      </c>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+    </row>
+    <row r="93" spans="1:8" ht="99">
+      <c r="A93" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B93" s="1">
+        <v>4</v>
+      </c>
+      <c r="C93" s="1">
+        <v>3</v>
+      </c>
+      <c r="D93" s="1">
+        <v>4</v>
+      </c>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+    </row>
+    <row r="94" spans="1:8" ht="115.5">
+      <c r="A94" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B94" s="1">
+        <v>4</v>
+      </c>
+      <c r="C94" s="1">
+        <v>4</v>
+      </c>
+      <c r="D94" s="1">
+        <v>4</v>
+      </c>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+    </row>
+    <row r="95" spans="1:8" ht="66">
+      <c r="A95" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="A79:H79"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="A2:H2"/>
@@ -2548,11 +2900,6 @@
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-24 16:45:41
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary_美化版.xlsx
+++ b/睡眠日记_Sleep_Diary_美化版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3EBEBF-74B2-4FE2-8307-30BDD7E7BE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9F3EDF-A803-4AF0-8C91-1D6C865B0989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="112">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -394,6 +394,15 @@
   </si>
   <si>
     <t>有 30 min</t>
+  </si>
+  <si>
+    <t>23：45</t>
+  </si>
+  <si>
+    <t>7：12</t>
+  </si>
+  <si>
+    <t>7：15</t>
   </si>
 </sst>
 </file>
@@ -545,7 +554,7 @@
     <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -559,7 +568,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -866,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="I91" sqref="I91"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -876,7 +885,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
@@ -888,7 +897,7 @@
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
@@ -1305,7 +1314,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="8"/>
@@ -1317,7 +1326,7 @@
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="8"/>
@@ -1731,7 +1740,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="8"/>
@@ -1743,7 +1752,7 @@
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="8"/>
@@ -2157,7 +2166,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="8"/>
@@ -2169,7 +2178,7 @@
       <c r="H59" s="9"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="8"/>
@@ -2583,7 +2592,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="13" t="s">
+      <c r="A79" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="8"/>
@@ -2645,8 +2654,12 @@
       <c r="D82" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E82" s="1"/>
-      <c r="F82" s="6"/>
+      <c r="E82" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="G82" s="6"/>
       <c r="H82" s="6"/>
     </row>
@@ -2663,8 +2676,12 @@
       <c r="D83" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E83" s="1"/>
-      <c r="F83" s="6"/>
+      <c r="E83" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G83" s="6"/>
       <c r="H83" s="1"/>
     </row>
@@ -2681,8 +2698,12 @@
       <c r="D84" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E84" s="1"/>
-      <c r="F84" s="6"/>
+      <c r="E84" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="G84" s="6"/>
       <c r="H84" s="1"/>
     </row>
@@ -2699,8 +2720,12 @@
       <c r="D85" s="6">
         <v>0.98611111111111116</v>
       </c>
-      <c r="E85" s="1"/>
-      <c r="F85" s="6"/>
+      <c r="E85" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>109</v>
+      </c>
       <c r="G85" s="6"/>
       <c r="H85" s="1"/>
     </row>
@@ -2717,8 +2742,12 @@
       <c r="D86" s="1">
         <v>5</v>
       </c>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
+      <c r="E86" s="1">
+        <v>0</v>
+      </c>
+      <c r="F86" s="1">
+        <v>60</v>
+      </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
@@ -2735,8 +2764,12 @@
       <c r="D87" s="1">
         <v>1</v>
       </c>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
+      <c r="E87" s="1">
+        <v>0</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0</v>
+      </c>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
@@ -2753,8 +2786,12 @@
       <c r="D88" s="1">
         <v>3</v>
       </c>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
+      <c r="E88" s="1">
+        <v>0</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0</v>
+      </c>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
     </row>
@@ -2771,8 +2808,12 @@
       <c r="D89" s="1">
         <v>480</v>
       </c>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
+      <c r="E89" s="1">
+        <v>480</v>
+      </c>
+      <c r="F89" s="1">
+        <v>480</v>
+      </c>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
     </row>
@@ -2789,8 +2830,12 @@
       <c r="D90" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
+      <c r="E90" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
     </row>
@@ -2807,8 +2852,12 @@
       <c r="D91" s="1">
         <v>25</v>
       </c>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
+      <c r="E91" s="1">
+        <v>0</v>
+      </c>
+      <c r="F91" s="1">
+        <v>60</v>
+      </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
     </row>
@@ -2825,8 +2874,12 @@
       <c r="D92" s="1">
         <v>4</v>
       </c>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
+      <c r="E92" s="1">
+        <v>4</v>
+      </c>
+      <c r="F92" s="1">
+        <v>3</v>
+      </c>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
@@ -2843,8 +2896,12 @@
       <c r="D93" s="1">
         <v>4</v>
       </c>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
+      <c r="E93" s="1">
+        <v>4</v>
+      </c>
+      <c r="F93" s="1">
+        <v>4</v>
+      </c>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
     </row>
@@ -2861,8 +2918,12 @@
       <c r="D94" s="1">
         <v>4</v>
       </c>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
+      <c r="E94" s="1">
+        <v>4</v>
+      </c>
+      <c r="F94" s="1">
+        <v>3</v>
+      </c>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
     </row>
@@ -2879,27 +2940,31 @@
       <c r="D95" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
+      <c r="E95" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A2:H2"/>
     <mergeCell ref="A79:H79"/>
     <mergeCell ref="B80:H80"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="A60:H60"/>
     <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>